<commit_message>
Changed randomized test world
</commit_message>
<xml_diff>
--- a/ExperimentResults/ResultStats.xlsx
+++ b/ExperimentResults/ResultStats.xlsx
@@ -224,9 +224,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -257,9 +257,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -597,9 +597,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -656,9 +656,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -699,9 +699,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -732,7 +732,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -773,20 +776,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average</a:t>
+              <a:t>Average Execution Time Adjusted for Failure Rate (ms)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Execution Time Adjusted for Failure Rate (ms)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -811,9 +809,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1151,9 +1149,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1210,9 +1208,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1253,9 +1251,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1286,7 +1284,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1327,20 +1328,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average</a:t>
+              <a:t>Average Bias</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Bias</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1365,9 +1361,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1705,9 +1701,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1764,9 +1760,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1807,9 +1803,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1840,7 +1836,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -1881,20 +1880,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Percentage of time</a:t>
+              <a:t>Percentage of time bias was toward the end rather than the beginning</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> bias was toward the end rather than the beginning</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1919,9 +1913,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -2259,9 +2253,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2318,9 +2312,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2361,9 +2355,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -2394,7 +2388,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2435,9 +2432,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -2468,9 +2465,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -2808,9 +2805,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2868,9 +2865,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2911,9 +2908,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -2944,7 +2941,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2985,9 +2985,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -3018,9 +3018,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3358,9 +3358,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3417,9 +3417,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3460,9 +3460,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3493,7 +3493,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3534,9 +3537,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -3567,9 +3570,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3907,9 +3910,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3966,9 +3969,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -4009,9 +4012,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -4042,7 +4045,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -4083,9 +4089,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -4116,9 +4122,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -4456,9 +4462,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -4515,9 +4521,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -4558,9 +4564,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -4591,7 +4597,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -4632,9 +4641,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -4665,9 +4674,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -5005,9 +5014,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -5064,9 +5073,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -5107,9 +5116,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -5140,7 +5149,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Helvetica" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -10581,7 +10593,7 @@
   <dimension ref="A2:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+      <selection activeCell="Z58" sqref="Z58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>